<commit_message>
add input/output columns to sugar templates
</commit_message>
<xml_diff>
--- a/templates/community/RPTU/RPTU_PP_SugarExtraction.xlsx
+++ b/templates/community/RPTU/RPTU_PP_SugarExtraction.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB71F28-6103-4C68-A8BF-36441FA1220A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="18000" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="isa_template" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="SugarExtraction" state="visible" r:id="rId5"/>
+    <sheet name="isa_template" sheetId="1" r:id="rId1"/>
+    <sheet name="SugarExtraction" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -163,19 +167,31 @@
   </si>
   <si>
     <t>https://bioregistry.io/UO:0000027</t>
+  </si>
+  <si>
+    <t>Input [Sample Name]</t>
+  </si>
+  <si>
+    <t>PlantHarvest</t>
+  </si>
+  <si>
+    <t>Output [Sample Name]</t>
+  </si>
+  <si>
+    <t>PlantSugarExtract</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,8 +234,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:H2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:H2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="annotationTable" displayName="annotationTable" ref="A1:J2">
+  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -228,16 +244,20 @@
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Parameter [Vortex Mixer]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Unit" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Term Source REF (NCIT:C29544)" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Term Accession Number (NCIT:C29544)" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Parameter [Temperature]" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Unit " totalsRowFunction="none"/>
-    <tableColumn id="7" name="Term Source REF (NCIT:C25206)" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Term Accession Number (NCIT:C25206)" totalsRowFunction="none"/>
+  <tableColumns count="10">
+    <tableColumn id="9" xr3:uid="{3CA674E2-D90D-4438-A606-DE58CBFA21DB}" name="Input [Sample Name]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Parameter [Vortex Mixer]" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Unit"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Term Source REF (NCIT:C29544)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Term Accession Number (NCIT:C29544)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter [Temperature]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit "/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Term Source REF (NCIT:C25206)"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Term Accession Number (NCIT:C25206)"/>
+    <tableColumn id="10" xr3:uid="{604293FC-67F5-4DB6-847E-30538A9D8CC0}" name="Output [Sample Name]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -539,16 +559,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="44.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -556,7 +584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -564,7 +592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -572,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -580,7 +608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -588,7 +616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -596,52 +624,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -649,7 +677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -657,117 +685,134 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>49</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>